<commit_message>
fix latency units in report sheets
</commit_message>
<xml_diff>
--- a/group-reports/tables/shahriar-1-2-tests-first-results-test-1.xlsx
+++ b/group-reports/tables/shahriar-1-2-tests-first-results-test-1.xlsx
@@ -579,7 +579,7 @@
       </c>
       <c r="O2" s="1" t="inlineStr">
         <is>
-          <t>Utility</t>
+          <t>Utility (Percent)</t>
         </is>
       </c>
     </row>
@@ -626,17 +626,17 @@
       </c>
       <c r="I3" s="1" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>60 msec</t>
         </is>
       </c>
       <c r="J3" s="1" t="inlineStr">
         <is>
-          <t>5318</t>
+          <t>5318 msec</t>
         </is>
       </c>
       <c r="K3" s="1" t="inlineStr">
         <is>
-          <t>2794.55</t>
+          <t>2794.55 msec</t>
         </is>
       </c>
       <c r="L3" s="1" t="inlineStr">
@@ -703,17 +703,17 @@
       </c>
       <c r="I4" s="1" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>40 msec</t>
         </is>
       </c>
       <c r="J4" s="1" t="inlineStr">
         <is>
-          <t>5174</t>
+          <t>5174 msec</t>
         </is>
       </c>
       <c r="K4" s="1" t="inlineStr">
         <is>
-          <t>2794.47</t>
+          <t>2794.47 msec</t>
         </is>
       </c>
       <c r="L4" s="1" t="inlineStr">
@@ -780,17 +780,17 @@
       </c>
       <c r="I5" s="1" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>42 msec</t>
         </is>
       </c>
       <c r="J5" s="1" t="inlineStr">
         <is>
-          <t>5251</t>
+          <t>5251 msec</t>
         </is>
       </c>
       <c r="K5" s="1" t="inlineStr">
         <is>
-          <t>2794.26</t>
+          <t>2794.26 msec</t>
         </is>
       </c>
       <c r="L5" s="1" t="inlineStr">
@@ -857,17 +857,17 @@
       </c>
       <c r="I6" s="1" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>77 msec</t>
         </is>
       </c>
       <c r="J6" s="1" t="inlineStr">
         <is>
-          <t>5269</t>
+          <t>5269 msec</t>
         </is>
       </c>
       <c r="K6" s="1" t="inlineStr">
         <is>
-          <t>2794.38</t>
+          <t>2794.38 msec</t>
         </is>
       </c>
       <c r="L6" s="1" t="inlineStr">
@@ -934,17 +934,17 @@
       </c>
       <c r="I7" s="1" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>60 msec</t>
         </is>
       </c>
       <c r="J7" s="1" t="inlineStr">
         <is>
-          <t>5154</t>
+          <t>5154 msec</t>
         </is>
       </c>
       <c r="K7" s="1" t="inlineStr">
         <is>
-          <t>2794.22</t>
+          <t>2794.22 msec</t>
         </is>
       </c>
       <c r="L7" s="1" t="inlineStr">
@@ -1011,17 +1011,17 @@
       </c>
       <c r="I8" s="1" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>77 msec</t>
         </is>
       </c>
       <c r="J8" s="1" t="inlineStr">
         <is>
-          <t>5299</t>
+          <t>5299 msec</t>
         </is>
       </c>
       <c r="K8" s="1" t="inlineStr">
         <is>
-          <t>2794.35</t>
+          <t>2794.35 msec</t>
         </is>
       </c>
       <c r="L8" s="1" t="inlineStr">
@@ -1088,17 +1088,17 @@
       </c>
       <c r="I9" s="1" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>30 msec</t>
         </is>
       </c>
       <c r="J9" s="1" t="inlineStr">
         <is>
-          <t>5266</t>
+          <t>5266 msec</t>
         </is>
       </c>
       <c r="K9" s="1" t="inlineStr">
         <is>
-          <t>2794.35</t>
+          <t>2794.35 msec</t>
         </is>
       </c>
       <c r="L9" s="1" t="inlineStr">
@@ -1165,17 +1165,17 @@
       </c>
       <c r="I10" s="1" t="inlineStr">
         <is>
-          <t>70</t>
+          <t>70 msec</t>
         </is>
       </c>
       <c r="J10" s="1" t="inlineStr">
         <is>
-          <t>5239</t>
+          <t>5239 msec</t>
         </is>
       </c>
       <c r="K10" s="1" t="inlineStr">
         <is>
-          <t>2794.30</t>
+          <t>2794.30 msec</t>
         </is>
       </c>
       <c r="L10" s="1" t="inlineStr">
@@ -1242,17 +1242,17 @@
       </c>
       <c r="I11" s="1" t="inlineStr">
         <is>
-          <t>85</t>
+          <t>85 msec</t>
         </is>
       </c>
       <c r="J11" s="1" t="inlineStr">
         <is>
-          <t>5263</t>
+          <t>5263 msec</t>
         </is>
       </c>
       <c r="K11" s="1" t="inlineStr">
         <is>
-          <t>2794.28</t>
+          <t>2794.28 msec</t>
         </is>
       </c>
       <c r="L11" s="1" t="inlineStr">
@@ -1319,17 +1319,17 @@
       </c>
       <c r="I12" s="1" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>56 msec</t>
         </is>
       </c>
       <c r="J12" s="1" t="inlineStr">
         <is>
-          <t>5270</t>
+          <t>5270 msec</t>
         </is>
       </c>
       <c r="K12" s="1" t="inlineStr">
         <is>
-          <t>2794.33</t>
+          <t>2794.33 msec</t>
         </is>
       </c>
       <c r="L12" s="1" t="inlineStr">
@@ -1396,17 +1396,17 @@
       </c>
       <c r="I13" s="1" t="inlineStr">
         <is>
-          <t>91</t>
+          <t>91 msec</t>
         </is>
       </c>
       <c r="J13" s="1" t="inlineStr">
         <is>
-          <t>5255</t>
+          <t>5255 msec</t>
         </is>
       </c>
       <c r="K13" s="1" t="inlineStr">
         <is>
-          <t>2794.32</t>
+          <t>2794.32 msec</t>
         </is>
       </c>
       <c r="L13" s="1" t="inlineStr">
@@ -1473,17 +1473,17 @@
       </c>
       <c r="I14" s="1" t="inlineStr">
         <is>
-          <t>59</t>
+          <t>59 msec</t>
         </is>
       </c>
       <c r="J14" s="1" t="inlineStr">
         <is>
-          <t>5154</t>
+          <t>5154 msec</t>
         </is>
       </c>
       <c r="K14" s="1" t="inlineStr">
         <is>
-          <t>2794.41</t>
+          <t>2794.41 msec</t>
         </is>
       </c>
       <c r="L14" s="1" t="inlineStr">
@@ -1550,17 +1550,17 @@
       </c>
       <c r="I15" s="1" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>37 msec</t>
         </is>
       </c>
       <c r="J15" s="1" t="inlineStr">
         <is>
-          <t>5234</t>
+          <t>5234 msec</t>
         </is>
       </c>
       <c r="K15" s="1" t="inlineStr">
         <is>
-          <t>2794.27</t>
+          <t>2794.27 msec</t>
         </is>
       </c>
       <c r="L15" s="1" t="inlineStr">

</xml_diff>